<commit_message>
update with newest sounds and cueing
</commit_message>
<xml_diff>
--- a/sequences/soundcheck.xlsx
+++ b/sequences/soundcheck.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
   <si>
     <t>word</t>
   </si>
@@ -77,6 +77,93 @@
   </si>
   <si>
     <t>vorsichtig</t>
+  </si>
+  <si>
+    <t>Abenteuer</t>
+  </si>
+  <si>
+    <t>angenehm</t>
+  </si>
+  <si>
+    <t>bewirken</t>
+  </si>
+  <si>
+    <t>Erdbeere</t>
+  </si>
+  <si>
+    <t>gefährlich</t>
+  </si>
+  <si>
+    <t>harmonisch</t>
+  </si>
+  <si>
+    <t>Kanister</t>
+  </si>
+  <si>
+    <t>Laterne</t>
+  </si>
+  <si>
+    <t>Maschine</t>
+  </si>
+  <si>
+    <t>notwendig</t>
+  </si>
+  <si>
+    <t>Operette</t>
+  </si>
+  <si>
+    <t>Paprika</t>
+  </si>
+  <si>
+    <t>Qualität</t>
+  </si>
+  <si>
+    <t>reparieren</t>
+  </si>
+  <si>
+    <t>Schokolade</t>
+  </si>
+  <si>
+    <t>Telefonat</t>
+  </si>
+  <si>
+    <t>Urlauber</t>
+  </si>
+  <si>
+    <t>verlassen</t>
+  </si>
+  <si>
+    <t>wunderbar</t>
+  </si>
+  <si>
+    <t>Zauberei</t>
+  </si>
+  <si>
+    <t>Apfelsine</t>
+  </si>
+  <si>
+    <t>Banane</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>dynamisch</t>
+  </si>
+  <si>
+    <t>Elefant</t>
+  </si>
+  <si>
+    <t>Familie</t>
+  </si>
+  <si>
+    <t>Gemüsefach</t>
+  </si>
+  <si>
+    <t>intelligent</t>
+  </si>
+  <si>
+    <t>Journalist</t>
   </si>
 </sst>
 </file>
@@ -474,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -603,6 +690,336 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>